<commit_message>
New round of calibration and First Round of Beads
</commit_message>
<xml_diff>
--- a/X2110-Camera/100x/cal3/calc.xlsx
+++ b/X2110-Camera/100x/cal3/calc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
   <si>
     <t>pixel</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>coef med</t>
+  </si>
+  <si>
+    <t>pixel disp</t>
   </si>
 </sst>
 </file>
@@ -202,13 +205,13 @@
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10086,22 +10089,22 @@
   <dimension ref="C2:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18:N21"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C2" s="9"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="16"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C3" s="10"/>
@@ -10167,7 +10170,7 @@
         <v>8</v>
       </c>
       <c r="S4" s="1">
-        <f>_xlfn.STDEV.P(G4,G11,G18,G25,G32,N4,N11,N18,N25)</f>
+        <f>_xlfn.STDEV.P(G4,G11,G18,G25,G32,N4,N11,N18)</f>
         <v>4.4335066291206738E-5</v>
       </c>
       <c r="U4" s="3">
@@ -10207,14 +10210,14 @@
         <v>9</v>
       </c>
       <c r="Q5" s="11">
-        <f t="shared" ref="Q5:Q7" si="0">(G5+G12+G19+G26+G33+N5+N12+N19)/8</f>
+        <f>(G5+G12+G19+G26+G33+N5+N12+N19)/8</f>
         <v>4.2605426575000001E-2</v>
       </c>
       <c r="R5" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="16">
-        <f t="shared" ref="S5:S7" si="1">_xlfn.STDEV.P(G5,G12,G19,G26,G33,N5,N12,N19,N26)</f>
+      <c r="S5" s="14">
+        <f t="shared" ref="S5:S7" si="0">_xlfn.STDEV.P(G5,G12,G19,G26,G33,N5,N12,N19,N26)</f>
         <v>3.8273339655753857E-3</v>
       </c>
     </row>
@@ -10250,14 +10253,14 @@
         <v>10</v>
       </c>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q5:Q7" si="1">(G6+G13+G20+G27+G34+N6+N13+N20)/8</f>
         <v>5.0555047675000004</v>
       </c>
       <c r="R6" t="s">
         <v>10</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1216882266870474</v>
       </c>
     </row>
@@ -10293,28 +10296,28 @@
         <v>11</v>
       </c>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>680</v>
       </c>
       <c r="R7" t="s">
         <v>11</v>
       </c>
       <c r="S7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="16"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
@@ -10334,8 +10337,11 @@
       <c r="L10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q10">
-        <v>4.7898776511111119E-4</v>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:21" x14ac:dyDescent="0.25">
@@ -10369,6 +10375,13 @@
       <c r="O11" t="s">
         <v>8</v>
       </c>
+      <c r="Q11">
+        <v>-30</v>
+      </c>
+      <c r="R11" s="3">
+        <f>Q11^3*$Q$4 + Q11^2*$Q$5 + Q11*$Q$6 + $Q$7</f>
+        <v>561.57531822875001</v>
+      </c>
     </row>
     <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
@@ -10401,6 +10414,13 @@
       <c r="O12" t="s">
         <v>9</v>
       </c>
+      <c r="Q12">
+        <v>-20</v>
+      </c>
+      <c r="R12" s="3">
+        <f>Q12^3*$Q$4 + Q12^2*$Q$5 + Q12*$Q$6 + $Q$7</f>
+        <v>594.41965374999995</v>
+      </c>
     </row>
     <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
@@ -10433,6 +10453,13 @@
       <c r="O13" t="s">
         <v>10</v>
       </c>
+      <c r="Q13">
+        <v>-32</v>
+      </c>
+      <c r="R13" s="3">
+        <f>Q13^3*$Q$4 + Q13^2*$Q$5 + Q13*$Q$6 + $Q$7</f>
+        <v>555.65692566591997</v>
+      </c>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
@@ -10468,15 +10495,15 @@
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="16"/>
       <c r="J16" s="9"/>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L16" s="15"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
@@ -10628,13 +10655,13 @@
     </row>
     <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="16"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="16"/>
     </row>
     <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="10"/>
@@ -10737,10 +10764,10 @@
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="16"/>
     </row>
     <row r="31" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C31" s="10"/>

</xml_diff>